<commit_message>
Sample program has been added
</commit_message>
<xml_diff>
--- a/ROM/Address Map.xlsx
+++ b/ROM/Address Map.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\@Development\8-Bit Cpu\ROM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37A63DE-B0C6-400C-ADB0-AF570BB30979}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6714E8AB-6A37-4F9F-B8E2-1C67F3245F99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FF26AF99-B2FA-4DE0-9A0B-DE1EB2D813C3}"/>
   </bookViews>
@@ -31,14 +31,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
   <si>
     <t>Value Binary</t>
   </si>
   <si>
-    <t>Fetch</t>
-  </si>
-  <si>
     <t>LDA</t>
   </si>
   <si>
@@ -63,9 +60,6 @@
     <t>AI</t>
   </si>
   <si>
-    <t>AO</t>
-  </si>
-  <si>
     <t>BIT 0</t>
   </si>
   <si>
@@ -130,6 +124,12 @@
   </si>
   <si>
     <t>T0</t>
+  </si>
+  <si>
+    <t>BI</t>
+  </si>
+  <si>
+    <t>Cycles</t>
   </si>
 </sst>
 </file>
@@ -386,7 +386,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -412,29 +412,17 @@
     <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -451,17 +439,20 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -486,14 +477,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
+          <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
+          <bgColor theme="6" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -814,10 +805,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFB10C3D-75E5-4409-9E10-E5591CCD00D1}">
-  <dimension ref="E4:Q36"/>
+  <dimension ref="E3:Q35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -831,411 +822,450 @@
     <col min="20" max="22" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="3" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E3" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16"/>
+    </row>
     <row r="4" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+    </row>
+    <row r="5" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+    </row>
+    <row r="6" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E6" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="17"/>
+      <c r="G6" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18"/>
+    </row>
+    <row r="7" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q7" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="5:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q8" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="20"/>
-    </row>
-    <row r="5" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="20"/>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="20"/>
-    </row>
-    <row r="6" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="20"/>
-      <c r="O6" s="20"/>
-      <c r="P6" s="20"/>
-      <c r="Q6" s="20"/>
-    </row>
-    <row r="7" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E7" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="21"/>
-      <c r="G7" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="H7" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="I7" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="J7" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="22"/>
-      <c r="O7" s="22"/>
-      <c r="P7" s="22"/>
-      <c r="Q7" s="22"/>
-    </row>
-    <row r="8" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="L8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="M8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="N8" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="O8" s="5" t="s">
+    </row>
+    <row r="9" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E9" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2" t="str">
+        <f>DEC2BIN(H9,8)</f>
+        <v>00000000</v>
+      </c>
+      <c r="J9" s="9">
+        <v>1</v>
+      </c>
+      <c r="K9" s="9">
+        <v>1</v>
+      </c>
+      <c r="L9" s="9">
+        <v>0</v>
+      </c>
+      <c r="M9" s="9">
+        <v>0</v>
+      </c>
+      <c r="N9" s="9">
+        <v>0</v>
+      </c>
+      <c r="O9" s="9">
+        <v>0</v>
+      </c>
+      <c r="P9" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E10" s="22"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="P8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q8" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="5:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="M9" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="N9" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="O9" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="P9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q9" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E10" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="H10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" s="2" t="str">
         <f>DEC2BIN(H10,8)</f>
-        <v>00000000</v>
-      </c>
-      <c r="J10" s="24">
-        <v>1</v>
-      </c>
-      <c r="K10" s="24">
-        <v>1</v>
-      </c>
-      <c r="L10" s="24">
-        <v>0</v>
-      </c>
-      <c r="M10" s="24">
-        <v>0</v>
-      </c>
-      <c r="N10" s="24">
-        <v>0</v>
-      </c>
-      <c r="O10" s="24">
-        <v>0</v>
-      </c>
-      <c r="P10" s="24">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="24">
+        <v>00000001</v>
+      </c>
+      <c r="J10" s="9">
+        <v>0</v>
+      </c>
+      <c r="K10" s="9">
+        <v>0</v>
+      </c>
+      <c r="L10" s="9">
+        <v>0</v>
+      </c>
+      <c r="M10" s="9">
+        <v>0</v>
+      </c>
+      <c r="N10" s="9">
+        <v>1</v>
+      </c>
+      <c r="O10" s="9">
+        <v>0</v>
+      </c>
+      <c r="P10" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E11" s="10"/>
-      <c r="F11" s="16"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H11" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I11" s="2" t="str">
         <f>DEC2BIN(H11,8)</f>
-        <v>00000001</v>
-      </c>
-      <c r="J11" s="24">
-        <v>0</v>
-      </c>
-      <c r="K11" s="24">
-        <v>0</v>
-      </c>
-      <c r="L11" s="24">
-        <v>0</v>
-      </c>
-      <c r="M11" s="24">
-        <v>0</v>
-      </c>
-      <c r="N11" s="24">
-        <v>1</v>
-      </c>
-      <c r="O11" s="24">
-        <v>0</v>
-      </c>
-      <c r="P11" s="24">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="24">
+        <v>00000010</v>
+      </c>
+      <c r="J11" s="9">
+        <v>0</v>
+      </c>
+      <c r="K11" s="9">
+        <v>0</v>
+      </c>
+      <c r="L11" s="9">
+        <v>1</v>
+      </c>
+      <c r="M11" s="9">
+        <v>1</v>
+      </c>
+      <c r="N11" s="9">
+        <v>0</v>
+      </c>
+      <c r="O11" s="9">
+        <v>0</v>
+      </c>
+      <c r="P11" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E12" s="10"/>
-      <c r="F12" s="16"/>
+      <c r="E12" s="24" t="str">
+        <f>DEC2BIN(0, 8)</f>
+        <v>00000000</v>
+      </c>
+      <c r="F12" s="22"/>
       <c r="G12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="2">
+        <v>3</v>
+      </c>
+      <c r="I12" s="10" t="str">
+        <f t="shared" ref="I12:I35" si="0">DEC2BIN(H12,8)</f>
+        <v>00000011</v>
+      </c>
+      <c r="J12" s="9">
+        <v>0</v>
+      </c>
+      <c r="K12" s="9">
+        <v>1</v>
+      </c>
+      <c r="L12" s="9">
+        <v>0</v>
+      </c>
+      <c r="M12" s="9">
+        <v>0</v>
+      </c>
+      <c r="N12" s="9">
+        <v>0</v>
+      </c>
+      <c r="O12" s="9">
+        <v>1</v>
+      </c>
+      <c r="P12" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H12" s="2">
-        <v>2</v>
-      </c>
-      <c r="I12" s="2" t="str">
-        <f>DEC2BIN(H12,8)</f>
-        <v>00000010</v>
-      </c>
-      <c r="J12" s="24">
-        <v>0</v>
-      </c>
-      <c r="K12" s="24">
-        <v>0</v>
-      </c>
-      <c r="L12" s="24">
-        <v>1</v>
-      </c>
-      <c r="M12" s="24">
-        <v>1</v>
-      </c>
-      <c r="N12" s="24">
-        <v>0</v>
-      </c>
-      <c r="O12" s="24">
-        <v>0</v>
-      </c>
-      <c r="P12" s="24">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E13" s="10"/>
-      <c r="F13" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="G13" s="3" t="s">
+      <c r="H13" s="2">
+        <v>4</v>
+      </c>
+      <c r="I13" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>00000100</v>
+      </c>
+      <c r="J13" s="9">
+        <v>0</v>
+      </c>
+      <c r="K13" s="9">
+        <v>0</v>
+      </c>
+      <c r="L13" s="9">
+        <v>1</v>
+      </c>
+      <c r="M13" s="9">
+        <v>0</v>
+      </c>
+      <c r="N13" s="9">
+        <v>0</v>
+      </c>
+      <c r="O13" s="9">
+        <v>0</v>
+      </c>
+      <c r="P13" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H13" s="2">
-        <v>3</v>
-      </c>
-      <c r="I13" s="25" t="str">
-        <f t="shared" ref="I13:I36" si="0">DEC2BIN(H13,8)</f>
-        <v>00000011</v>
-      </c>
-      <c r="J13" s="24">
-        <v>0</v>
-      </c>
-      <c r="K13" s="24">
-        <v>1</v>
-      </c>
-      <c r="L13" s="24">
-        <v>0</v>
-      </c>
-      <c r="M13" s="24">
-        <v>0</v>
-      </c>
-      <c r="N13" s="24">
-        <v>0</v>
-      </c>
-      <c r="O13" s="24">
-        <v>1</v>
-      </c>
-      <c r="P13" s="24">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E14" s="10"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="H14" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I14" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>00000100</v>
-      </c>
-      <c r="J14" s="24">
-        <v>0</v>
-      </c>
-      <c r="K14" s="24">
-        <v>0</v>
-      </c>
-      <c r="L14" s="24">
-        <v>1</v>
-      </c>
-      <c r="M14" s="24">
-        <v>0</v>
-      </c>
-      <c r="N14" s="24">
-        <v>0</v>
-      </c>
-      <c r="O14" s="24">
-        <v>0</v>
-      </c>
-      <c r="P14" s="24">
-        <v>1</v>
-      </c>
-      <c r="Q14" s="24">
+        <v>00000101</v>
+      </c>
+      <c r="J14" s="9">
+        <v>0</v>
+      </c>
+      <c r="K14" s="9">
+        <v>0</v>
+      </c>
+      <c r="L14" s="9">
+        <v>0</v>
+      </c>
+      <c r="M14" s="9">
+        <v>0</v>
+      </c>
+      <c r="N14" s="9">
+        <v>0</v>
+      </c>
+      <c r="O14" s="9">
+        <v>0</v>
+      </c>
+      <c r="P14" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E15" s="10"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H15" s="2">
-        <v>5</v>
-      </c>
-      <c r="I15" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>00000101</v>
-      </c>
-      <c r="J15" s="24">
-        <v>0</v>
-      </c>
-      <c r="K15" s="24">
-        <v>0</v>
-      </c>
-      <c r="L15" s="24">
-        <v>0</v>
-      </c>
-      <c r="M15" s="24">
-        <v>0</v>
-      </c>
-      <c r="N15" s="24">
-        <v>0</v>
-      </c>
-      <c r="O15" s="24">
-        <v>0</v>
-      </c>
-      <c r="P15" s="24">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="24">
-        <v>0</v>
-      </c>
+      <c r="E15" s="13"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="15"/>
     </row>
     <row r="16" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E16" s="17"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18"/>
-      <c r="N16" s="18"/>
-      <c r="O16" s="18"/>
-      <c r="P16" s="18"/>
-      <c r="Q16" s="19"/>
-    </row>
-    <row r="17" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E17" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="G17" s="7" t="s">
+      <c r="E16" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H17" s="1">
+      <c r="G16" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="1">
         <v>8</v>
       </c>
-      <c r="I17" s="1" t="str">
+      <c r="I16" s="1" t="str">
         <f t="shared" si="0"/>
         <v>00001000</v>
       </c>
+      <c r="J16" s="4">
+        <v>1</v>
+      </c>
+      <c r="K16" s="4">
+        <v>1</v>
+      </c>
+      <c r="L16" s="4">
+        <v>0</v>
+      </c>
+      <c r="M16" s="4">
+        <v>0</v>
+      </c>
+      <c r="N16" s="4">
+        <v>0</v>
+      </c>
+      <c r="O16" s="4">
+        <v>0</v>
+      </c>
+      <c r="P16" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E17" s="22"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="2">
+        <v>9</v>
+      </c>
+      <c r="I17" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>00001001</v>
+      </c>
       <c r="J17" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K17" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L17" s="4">
         <v>0</v>
@@ -1244,7 +1274,7 @@
         <v>0</v>
       </c>
       <c r="N17" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O17" s="4">
         <v>0</v>
@@ -1257,17 +1287,17 @@
       </c>
     </row>
     <row r="18" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E18" s="10"/>
-      <c r="F18" s="16"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="21"/>
       <c r="G18" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H18" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I18" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>00001001</v>
+        <v>00001010</v>
       </c>
       <c r="J18" s="4">
         <v>0</v>
@@ -1282,7 +1312,7 @@
         <v>1</v>
       </c>
       <c r="N18" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O18" s="4">
         <v>0</v>
@@ -1295,58 +1325,61 @@
       </c>
     </row>
     <row r="19" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E19" s="10"/>
-      <c r="F19" s="16"/>
+      <c r="E19" s="24" t="str">
+        <f>DEC2BIN(1, 8)</f>
+        <v>00000001</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>26</v>
+      </c>
       <c r="G19" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H19" s="2">
-        <v>10</v>
-      </c>
-      <c r="I19" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>00001010</v>
-      </c>
-      <c r="J19" s="4">
-        <v>0</v>
-      </c>
-      <c r="K19" s="4">
-        <v>1</v>
-      </c>
-      <c r="L19" s="4">
-        <v>0</v>
-      </c>
-      <c r="M19" s="4">
-        <v>0</v>
-      </c>
-      <c r="N19" s="4">
-        <v>0</v>
-      </c>
-      <c r="O19" s="4">
-        <v>1</v>
-      </c>
-      <c r="P19" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E20" s="10"/>
-      <c r="F20" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H20" s="2">
         <v>11</v>
       </c>
-      <c r="I20" s="26" t="str">
+      <c r="I19" s="11" t="str">
         <f t="shared" si="0"/>
         <v>00001011</v>
       </c>
+      <c r="J19" s="4">
+        <v>0</v>
+      </c>
+      <c r="K19" s="4">
+        <v>1</v>
+      </c>
+      <c r="L19" s="4">
+        <v>0</v>
+      </c>
+      <c r="M19" s="4">
+        <v>0</v>
+      </c>
+      <c r="N19" s="4">
+        <v>0</v>
+      </c>
+      <c r="O19" s="4">
+        <v>1</v>
+      </c>
+      <c r="P19" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="2">
+        <v>12</v>
+      </c>
+      <c r="I20" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>00001100</v>
+      </c>
       <c r="J20" s="4">
         <v>0</v>
       </c>
@@ -1366,24 +1399,24 @@
         <v>0</v>
       </c>
       <c r="P20" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q20" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E21" s="10"/>
-      <c r="F21" s="16"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
       <c r="G21" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H21" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I21" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>00001100</v>
+        <v>00001101</v>
       </c>
       <c r="J21" s="4">
         <v>0</v>
@@ -1411,89 +1444,89 @@
       </c>
     </row>
     <row r="22" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E22" s="10"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H22" s="2">
-        <v>13</v>
-      </c>
-      <c r="I22" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>00001101</v>
-      </c>
-      <c r="J22" s="4">
-        <v>0</v>
-      </c>
-      <c r="K22" s="4">
-        <v>0</v>
-      </c>
-      <c r="L22" s="4">
-        <v>0</v>
-      </c>
-      <c r="M22" s="4">
-        <v>0</v>
-      </c>
-      <c r="N22" s="4">
-        <v>0</v>
-      </c>
-      <c r="O22" s="4">
-        <v>0</v>
-      </c>
-      <c r="P22" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="4">
-        <v>0</v>
-      </c>
+      <c r="E22" s="13"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="14"/>
+      <c r="O22" s="14"/>
+      <c r="P22" s="14"/>
+      <c r="Q22" s="15"/>
     </row>
     <row r="23" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E23" s="17"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="18"/>
-      <c r="N23" s="18"/>
-      <c r="O23" s="18"/>
-      <c r="P23" s="18"/>
-      <c r="Q23" s="19"/>
-    </row>
-    <row r="24" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E24" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F24" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="G24" s="7" t="s">
+      <c r="E23" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H24" s="1">
+      <c r="G23" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H23" s="1">
         <v>14</v>
       </c>
-      <c r="I24" s="1" t="str">
+      <c r="I23" s="1" t="str">
         <f t="shared" si="0"/>
         <v>00001110</v>
       </c>
+      <c r="J23" s="4">
+        <v>1</v>
+      </c>
+      <c r="K23" s="4">
+        <v>1</v>
+      </c>
+      <c r="L23" s="4">
+        <v>0</v>
+      </c>
+      <c r="M23" s="4">
+        <v>0</v>
+      </c>
+      <c r="N23" s="4">
+        <v>0</v>
+      </c>
+      <c r="O23" s="4">
+        <v>0</v>
+      </c>
+      <c r="P23" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E24" s="22"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" s="1">
+        <v>15</v>
+      </c>
+      <c r="I24" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>00001111</v>
+      </c>
       <c r="J24" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K24" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L24" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M24" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N24" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O24" s="4">
         <v>0</v>
@@ -1506,35 +1539,35 @@
       </c>
     </row>
     <row r="25" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E25" s="10"/>
-      <c r="F25" s="16"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="21"/>
       <c r="G25" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H25" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I25" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>00001111</v>
+        <v>00010000</v>
       </c>
       <c r="J25" s="4">
         <v>0</v>
       </c>
       <c r="K25" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L25" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M25" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N25" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O25" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P25" s="4">
         <v>0</v>
@@ -1544,58 +1577,61 @@
       </c>
     </row>
     <row r="26" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E26" s="10"/>
-      <c r="F26" s="16"/>
+      <c r="E26" s="24" t="str">
+        <f>DEC2BIN(2, 8)</f>
+        <v>00000010</v>
+      </c>
+      <c r="F26" s="22" t="s">
+        <v>27</v>
+      </c>
       <c r="G26" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H26" s="1">
-        <v>16</v>
-      </c>
-      <c r="I26" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>00010000</v>
-      </c>
-      <c r="J26" s="4">
-        <v>0</v>
-      </c>
-      <c r="K26" s="4">
-        <v>1</v>
-      </c>
-      <c r="L26" s="4">
-        <v>0</v>
-      </c>
-      <c r="M26" s="4">
-        <v>0</v>
-      </c>
-      <c r="N26" s="4">
-        <v>0</v>
-      </c>
-      <c r="O26" s="4">
-        <v>1</v>
-      </c>
-      <c r="P26" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E27" s="10"/>
-      <c r="F27" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H27" s="1">
         <v>17</v>
       </c>
-      <c r="I27" s="26" t="str">
+      <c r="I26" s="11" t="str">
         <f t="shared" si="0"/>
         <v>00010001</v>
       </c>
+      <c r="J26" s="4">
+        <v>0</v>
+      </c>
+      <c r="K26" s="4">
+        <v>0</v>
+      </c>
+      <c r="L26" s="4">
+        <v>1</v>
+      </c>
+      <c r="M26" s="4">
+        <v>0</v>
+      </c>
+      <c r="N26" s="4">
+        <v>0</v>
+      </c>
+      <c r="O26" s="4">
+        <v>0</v>
+      </c>
+      <c r="P26" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H27" s="1">
+        <v>18</v>
+      </c>
+      <c r="I27" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>00010010</v>
+      </c>
       <c r="J27" s="4">
         <v>0</v>
       </c>
@@ -1603,7 +1639,7 @@
         <v>0</v>
       </c>
       <c r="L27" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M27" s="4">
         <v>0</v>
@@ -1615,24 +1651,24 @@
         <v>0</v>
       </c>
       <c r="P27" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q27" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E28" s="10"/>
-      <c r="F28" s="16"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
       <c r="G28" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H28" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I28" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>00010010</v>
+        <v>00010011</v>
       </c>
       <c r="J28" s="4">
         <v>0</v>
@@ -1660,75 +1696,75 @@
       </c>
     </row>
     <row r="29" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E29" s="10"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H29" s="1">
-        <v>19</v>
-      </c>
-      <c r="I29" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>00010011</v>
-      </c>
-      <c r="J29" s="4">
-        <v>0</v>
-      </c>
-      <c r="K29" s="4">
-        <v>0</v>
-      </c>
-      <c r="L29" s="4">
-        <v>0</v>
-      </c>
-      <c r="M29" s="4">
-        <v>0</v>
-      </c>
-      <c r="N29" s="4">
-        <v>0</v>
-      </c>
-      <c r="O29" s="4">
-        <v>0</v>
-      </c>
-      <c r="P29" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q29" s="4">
-        <v>0</v>
-      </c>
+      <c r="E29" s="13"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
+      <c r="K29" s="14"/>
+      <c r="L29" s="14"/>
+      <c r="M29" s="14"/>
+      <c r="N29" s="14"/>
+      <c r="O29" s="14"/>
+      <c r="P29" s="14"/>
+      <c r="Q29" s="15"/>
     </row>
     <row r="30" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E30" s="17"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="18"/>
-      <c r="J30" s="18"/>
-      <c r="K30" s="18"/>
-      <c r="L30" s="18"/>
-      <c r="M30" s="18"/>
-      <c r="N30" s="18"/>
-      <c r="O30" s="18"/>
-      <c r="P30" s="18"/>
-      <c r="Q30" s="19"/>
-    </row>
-    <row r="31" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E31" s="9" t="s">
+      <c r="E30" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="F30" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="G30" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F31" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="H31" s="2">
+      <c r="H30" s="2">
         <v>20</v>
       </c>
-      <c r="I31" s="27" t="str">
+      <c r="I30" s="12" t="str">
         <f t="shared" si="0"/>
         <v>00010100</v>
       </c>
+      <c r="J30" s="8">
+        <v>0</v>
+      </c>
+      <c r="K30" s="8">
+        <v>0</v>
+      </c>
+      <c r="L30" s="8">
+        <v>0</v>
+      </c>
+      <c r="M30" s="8">
+        <v>0</v>
+      </c>
+      <c r="N30" s="8">
+        <v>0</v>
+      </c>
+      <c r="O30" s="8">
+        <v>0</v>
+      </c>
+      <c r="P30" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E31" s="22"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H31" s="2">
+        <v>21</v>
+      </c>
+      <c r="I31" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>00010101</v>
+      </c>
       <c r="J31" s="8">
         <v>0</v>
       </c>
@@ -1755,17 +1791,17 @@
       </c>
     </row>
     <row r="32" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E32" s="10"/>
-      <c r="F32" s="12"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="21"/>
       <c r="G32" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H32" s="2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I32" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>00010101</v>
+        <v>00010110</v>
       </c>
       <c r="J32" s="8">
         <v>0</v>
@@ -1793,17 +1829,20 @@
       </c>
     </row>
     <row r="33" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E33" s="10"/>
-      <c r="F33" s="12"/>
+      <c r="E33" s="24" t="str">
+        <f>DEC2BIN(3, 8)</f>
+        <v>00000011</v>
+      </c>
+      <c r="F33" s="22"/>
       <c r="G33" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H33" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I33" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>00010110</v>
+        <v>00010111</v>
       </c>
       <c r="J33" s="8">
         <v>0</v>
@@ -1831,17 +1870,17 @@
       </c>
     </row>
     <row r="34" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E34" s="10"/>
-      <c r="F34" s="13"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
       <c r="G34" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H34" s="2">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I34" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>00010111</v>
+        <v>00011000</v>
       </c>
       <c r="J34" s="8">
         <v>0</v>
@@ -1869,17 +1908,17 @@
       </c>
     </row>
     <row r="35" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E35" s="10"/>
-      <c r="F35" s="13"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
       <c r="G35" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H35" s="2">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I35" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>00011000</v>
+        <v>00011001</v>
       </c>
       <c r="J35" s="8">
         <v>0</v>
@@ -1906,97 +1945,59 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E36" s="10"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H36" s="2">
-        <v>25</v>
-      </c>
-      <c r="I36" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>00011001</v>
-      </c>
-      <c r="J36" s="8">
-        <v>0</v>
-      </c>
-      <c r="K36" s="8">
-        <v>0</v>
-      </c>
-      <c r="L36" s="8">
-        <v>0</v>
-      </c>
-      <c r="M36" s="8">
-        <v>0</v>
-      </c>
-      <c r="N36" s="8">
-        <v>0</v>
-      </c>
-      <c r="O36" s="8">
-        <v>0</v>
-      </c>
-      <c r="P36" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q36" s="8">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="20">
-    <mergeCell ref="E23:Q23"/>
-    <mergeCell ref="E4:Q6"/>
-    <mergeCell ref="E30:Q30"/>
-    <mergeCell ref="E10:E15"/>
-    <mergeCell ref="E7:F9"/>
-    <mergeCell ref="E17:E22"/>
-    <mergeCell ref="F17:F19"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="E16:Q16"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="F13:F15"/>
-    <mergeCell ref="J7:Q7"/>
-    <mergeCell ref="I7:I9"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="E31:E36"/>
-    <mergeCell ref="F31:F36"/>
-    <mergeCell ref="E24:E29"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="F27:F29"/>
+  <mergeCells count="21">
+    <mergeCell ref="F9:F14"/>
+    <mergeCell ref="F16:F21"/>
+    <mergeCell ref="F23:F28"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="E16:E18"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="E23:E25"/>
+    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="F30:F35"/>
+    <mergeCell ref="E30:E32"/>
+    <mergeCell ref="E33:E35"/>
+    <mergeCell ref="E22:Q22"/>
+    <mergeCell ref="E3:Q5"/>
+    <mergeCell ref="E29:Q29"/>
+    <mergeCell ref="E6:F8"/>
+    <mergeCell ref="E15:Q15"/>
+    <mergeCell ref="J6:Q6"/>
+    <mergeCell ref="I6:I8"/>
+    <mergeCell ref="H6:H8"/>
+    <mergeCell ref="G6:G8"/>
+    <mergeCell ref="E9:E11"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="J10:Q15">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+  <conditionalFormatting sqref="J9:Q14">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J16:Q21 J23:Q28 J30:Q35">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J17:Q22 J24:Q29 J31:Q36">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>0</formula>
-    </cfRule>
   </conditionalFormatting>
   <dataValidations count="11">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Instruction:" prompt="Counter Out" sqref="J9" xr:uid="{A0954D8A-9790-41BF-AFCF-A3F6814EEAAF}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Instruction:" prompt="Memory Address Register In" sqref="K9" xr:uid="{0F47D54A-009D-48DF-B535-07EDF6183A02}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Instruction:" prompt="RAM Out" sqref="L9" xr:uid="{404A1873-2419-48E7-A1ED-2652D94585AE}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Instruction:" prompt="Instruction Register In" sqref="M9" xr:uid="{32B200C4-9B02-4F26-8C03-ECB518F03D48}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Instruction:" prompt="Counter Enabled_x000a_" sqref="N9" xr:uid="{1723EDCE-8B9C-4452-9F01-C6004BC68F5E}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Instruction:" prompt="Instruction Register Out" sqref="O9" xr:uid="{978199BB-A9C8-4546-88BB-8D04150D59C0}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Instruction:" prompt="Register A In" sqref="P9" xr:uid="{78960928-3245-42BA-BD7B-81A892A11758}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Instruction:" prompt="Register A Out" sqref="Q9" xr:uid="{438CDCA1-5791-4478-AB9D-BDCDC7D2B09B}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Instruction" prompt="Load to A Register" sqref="E10:E36" xr:uid="{1FB07C79-F2AE-4EBA-9CA0-77B10BDB2FC0}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Instruction " prompt="Fetch Cycle" sqref="F10:F12 F17:F19 F24:F26 F31:F33" xr:uid="{6D5BC8B1-0739-4E01-9DBE-1309CC76726D}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Instruction" prompt="Load value to Register A" sqref="F20:F23 F13:F15 F27:F30" xr:uid="{F93043F1-76DA-431B-860E-807A02D1E094}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Instruction:" prompt="Counter Out" sqref="J8" xr:uid="{A0954D8A-9790-41BF-AFCF-A3F6814EEAAF}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Instruction:" prompt="Memory Address Register In" sqref="K8" xr:uid="{0F47D54A-009D-48DF-B535-07EDF6183A02}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Instruction:" prompt="RAM Out" sqref="L8" xr:uid="{404A1873-2419-48E7-A1ED-2652D94585AE}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Instruction:" prompt="Instruction Register In" sqref="M8" xr:uid="{32B200C4-9B02-4F26-8C03-ECB518F03D48}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Instruction:" prompt="Counter Enabled_x000a_" sqref="N8" xr:uid="{1723EDCE-8B9C-4452-9F01-C6004BC68F5E}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Instruction:" prompt="Instruction Register Out" sqref="O8" xr:uid="{978199BB-A9C8-4546-88BB-8D04150D59C0}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Instruction:" prompt="Register A In" sqref="P8" xr:uid="{78960928-3245-42BA-BD7B-81A892A11758}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Instruction:" prompt="Register A Out" sqref="Q8" xr:uid="{438CDCA1-5791-4478-AB9D-BDCDC7D2B09B}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Instruction" prompt="Load to A Register" sqref="E9 E12 E15:E35" xr:uid="{1FB07C79-F2AE-4EBA-9CA0-77B10BDB2FC0}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Instruction " prompt="Fetch Cycle" sqref="F9:F11 F16:F18 F23:F25 F30:F32" xr:uid="{6D5BC8B1-0739-4E01-9DBE-1309CC76726D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Instruction" prompt="Load value to Register A" sqref="F19:F22 F26:F29" xr:uid="{F93043F1-76DA-431B-860E-807A02D1E094}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>